<commit_message>
1er avance de Save As y Save
</commit_message>
<xml_diff>
--- a/Saves/ae.xlsx
+++ b/Saves/ae.xlsx
@@ -467,11 +467,11 @@
         <v>12</v>
       </c>
       <c r="C2" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>1,2,3</t>
+          <t>1,,,2,,,3</t>
         </is>
       </c>
     </row>
@@ -500,172 +500,18 @@
           <t>44</t>
         </is>
       </c>
-      <c r="B1" t="inlineStr"/>
-      <c r="C1" t="inlineStr"/>
-      <c r="D1" t="inlineStr"/>
-      <c r="E1" t="inlineStr"/>
-      <c r="F1" t="inlineStr"/>
-      <c r="G1" t="inlineStr"/>
-      <c r="H1" t="inlineStr"/>
-      <c r="I1" t="inlineStr"/>
-      <c r="J1" t="inlineStr"/>
-      <c r="K1" t="inlineStr"/>
-      <c r="L1" t="inlineStr"/>
     </row>
-    <row r="2">
-      <c r="A2" t="inlineStr"/>
-      <c r="B2" t="inlineStr"/>
-      <c r="C2" t="inlineStr"/>
-      <c r="D2" t="inlineStr"/>
-      <c r="E2" t="inlineStr"/>
-      <c r="F2" t="inlineStr"/>
-      <c r="G2" t="inlineStr"/>
-      <c r="H2" t="inlineStr"/>
-      <c r="I2" t="inlineStr"/>
-      <c r="J2" t="inlineStr"/>
-      <c r="K2" t="inlineStr"/>
-      <c r="L2" t="inlineStr"/>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr"/>
-      <c r="B3" t="inlineStr"/>
-      <c r="C3" t="inlineStr"/>
-      <c r="D3" t="inlineStr"/>
-      <c r="E3" t="inlineStr"/>
-      <c r="F3" t="inlineStr"/>
-      <c r="G3" t="inlineStr"/>
-      <c r="H3" t="inlineStr"/>
-      <c r="I3" t="inlineStr"/>
-      <c r="J3" t="inlineStr"/>
-      <c r="K3" t="inlineStr"/>
-      <c r="L3" t="inlineStr"/>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr"/>
-      <c r="B4" t="inlineStr"/>
-      <c r="C4" t="inlineStr"/>
-      <c r="D4" t="inlineStr"/>
-      <c r="E4" t="inlineStr"/>
-      <c r="F4" t="inlineStr"/>
-      <c r="G4" t="inlineStr"/>
-      <c r="H4" t="inlineStr"/>
-      <c r="I4" t="inlineStr"/>
-      <c r="J4" t="inlineStr"/>
-      <c r="K4" t="inlineStr"/>
-      <c r="L4" t="inlineStr"/>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr"/>
-      <c r="B5" t="inlineStr"/>
-      <c r="C5" t="inlineStr"/>
-      <c r="D5" t="inlineStr"/>
-      <c r="E5" t="inlineStr"/>
-      <c r="F5" t="inlineStr"/>
-      <c r="G5" t="inlineStr"/>
-      <c r="H5" t="inlineStr"/>
-      <c r="I5" t="inlineStr"/>
-      <c r="J5" t="inlineStr"/>
-      <c r="K5" t="inlineStr"/>
-      <c r="L5" t="inlineStr"/>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr"/>
-      <c r="B6" t="inlineStr"/>
-      <c r="C6" t="inlineStr"/>
-      <c r="D6" t="inlineStr"/>
-      <c r="E6" t="inlineStr"/>
-      <c r="F6" t="inlineStr"/>
-      <c r="G6" t="inlineStr"/>
-      <c r="H6" t="inlineStr"/>
-      <c r="I6" t="inlineStr"/>
-      <c r="J6" t="inlineStr"/>
-      <c r="K6" t="inlineStr"/>
-      <c r="L6" t="inlineStr"/>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr"/>
-      <c r="B7" t="inlineStr"/>
-      <c r="C7" t="inlineStr"/>
-      <c r="D7" t="inlineStr"/>
-      <c r="E7" t="inlineStr"/>
-      <c r="F7" t="inlineStr"/>
-      <c r="G7" t="inlineStr"/>
-      <c r="H7" t="inlineStr"/>
-      <c r="I7" t="inlineStr"/>
-      <c r="J7" t="inlineStr"/>
-      <c r="K7" t="inlineStr"/>
-      <c r="L7" t="inlineStr"/>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr"/>
-      <c r="B8" t="inlineStr"/>
-      <c r="C8" t="inlineStr"/>
-      <c r="D8" t="inlineStr"/>
-      <c r="E8" t="inlineStr"/>
-      <c r="F8" t="inlineStr"/>
-      <c r="G8" t="inlineStr"/>
-      <c r="H8" t="inlineStr"/>
-      <c r="I8" t="inlineStr"/>
-      <c r="J8" t="inlineStr"/>
-      <c r="K8" t="inlineStr"/>
-      <c r="L8" t="inlineStr"/>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr"/>
-      <c r="B9" t="inlineStr"/>
-      <c r="C9" t="inlineStr"/>
-      <c r="D9" t="inlineStr"/>
-      <c r="E9" t="inlineStr"/>
-      <c r="F9" t="inlineStr"/>
-      <c r="G9" t="inlineStr"/>
-      <c r="H9" t="inlineStr"/>
-      <c r="I9" t="inlineStr"/>
-      <c r="J9" t="inlineStr"/>
-      <c r="K9" t="inlineStr"/>
-      <c r="L9" t="inlineStr"/>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr"/>
-      <c r="B10" t="inlineStr"/>
-      <c r="C10" t="inlineStr"/>
-      <c r="D10" t="inlineStr"/>
-      <c r="E10" t="inlineStr"/>
-      <c r="F10" t="inlineStr"/>
-      <c r="G10" t="inlineStr"/>
-      <c r="H10" t="inlineStr"/>
-      <c r="I10" t="inlineStr"/>
-      <c r="J10" t="inlineStr"/>
-      <c r="K10" t="inlineStr"/>
-      <c r="L10" t="inlineStr"/>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr"/>
-      <c r="B11" t="inlineStr"/>
-      <c r="C11" t="inlineStr"/>
-      <c r="D11" t="inlineStr"/>
-      <c r="E11" t="inlineStr"/>
-      <c r="F11" t="inlineStr"/>
-      <c r="G11" t="inlineStr"/>
-      <c r="H11" t="inlineStr"/>
-      <c r="I11" t="inlineStr"/>
-      <c r="J11" t="inlineStr"/>
-      <c r="K11" t="inlineStr"/>
-      <c r="L11" t="inlineStr"/>
-    </row>
-    <row r="12">
-      <c r="A12" t="inlineStr"/>
-      <c r="B12" t="inlineStr"/>
-      <c r="C12" t="inlineStr"/>
-      <c r="D12" t="inlineStr"/>
-      <c r="E12" t="inlineStr"/>
-      <c r="F12" t="inlineStr"/>
-      <c r="G12" t="inlineStr"/>
-      <c r="H12" t="inlineStr"/>
-      <c r="I12" t="inlineStr"/>
-      <c r="J12" t="inlineStr"/>
-      <c r="K12" t="inlineStr"/>
-      <c r="L12" t="inlineStr"/>
-    </row>
+    <row r="2"/>
+    <row r="3"/>
+    <row r="4"/>
+    <row r="5"/>
+    <row r="6"/>
+    <row r="7"/>
+    <row r="8"/>
+    <row r="9"/>
+    <row r="10"/>
+    <row r="11"/>
+    <row r="12"/>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
@@ -691,172 +537,18 @@
           <t>55</t>
         </is>
       </c>
-      <c r="B1" t="inlineStr"/>
-      <c r="C1" t="inlineStr"/>
-      <c r="D1" t="inlineStr"/>
-      <c r="E1" t="inlineStr"/>
-      <c r="F1" t="inlineStr"/>
-      <c r="G1" t="inlineStr"/>
-      <c r="H1" t="inlineStr"/>
-      <c r="I1" t="inlineStr"/>
-      <c r="J1" t="inlineStr"/>
-      <c r="K1" t="inlineStr"/>
-      <c r="L1" t="inlineStr"/>
     </row>
-    <row r="2">
-      <c r="A2" t="inlineStr"/>
-      <c r="B2" t="inlineStr"/>
-      <c r="C2" t="inlineStr"/>
-      <c r="D2" t="inlineStr"/>
-      <c r="E2" t="inlineStr"/>
-      <c r="F2" t="inlineStr"/>
-      <c r="G2" t="inlineStr"/>
-      <c r="H2" t="inlineStr"/>
-      <c r="I2" t="inlineStr"/>
-      <c r="J2" t="inlineStr"/>
-      <c r="K2" t="inlineStr"/>
-      <c r="L2" t="inlineStr"/>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr"/>
-      <c r="B3" t="inlineStr"/>
-      <c r="C3" t="inlineStr"/>
-      <c r="D3" t="inlineStr"/>
-      <c r="E3" t="inlineStr"/>
-      <c r="F3" t="inlineStr"/>
-      <c r="G3" t="inlineStr"/>
-      <c r="H3" t="inlineStr"/>
-      <c r="I3" t="inlineStr"/>
-      <c r="J3" t="inlineStr"/>
-      <c r="K3" t="inlineStr"/>
-      <c r="L3" t="inlineStr"/>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr"/>
-      <c r="B4" t="inlineStr"/>
-      <c r="C4" t="inlineStr"/>
-      <c r="D4" t="inlineStr"/>
-      <c r="E4" t="inlineStr"/>
-      <c r="F4" t="inlineStr"/>
-      <c r="G4" t="inlineStr"/>
-      <c r="H4" t="inlineStr"/>
-      <c r="I4" t="inlineStr"/>
-      <c r="J4" t="inlineStr"/>
-      <c r="K4" t="inlineStr"/>
-      <c r="L4" t="inlineStr"/>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr"/>
-      <c r="B5" t="inlineStr"/>
-      <c r="C5" t="inlineStr"/>
-      <c r="D5" t="inlineStr"/>
-      <c r="E5" t="inlineStr"/>
-      <c r="F5" t="inlineStr"/>
-      <c r="G5" t="inlineStr"/>
-      <c r="H5" t="inlineStr"/>
-      <c r="I5" t="inlineStr"/>
-      <c r="J5" t="inlineStr"/>
-      <c r="K5" t="inlineStr"/>
-      <c r="L5" t="inlineStr"/>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr"/>
-      <c r="B6" t="inlineStr"/>
-      <c r="C6" t="inlineStr"/>
-      <c r="D6" t="inlineStr"/>
-      <c r="E6" t="inlineStr"/>
-      <c r="F6" t="inlineStr"/>
-      <c r="G6" t="inlineStr"/>
-      <c r="H6" t="inlineStr"/>
-      <c r="I6" t="inlineStr"/>
-      <c r="J6" t="inlineStr"/>
-      <c r="K6" t="inlineStr"/>
-      <c r="L6" t="inlineStr"/>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr"/>
-      <c r="B7" t="inlineStr"/>
-      <c r="C7" t="inlineStr"/>
-      <c r="D7" t="inlineStr"/>
-      <c r="E7" t="inlineStr"/>
-      <c r="F7" t="inlineStr"/>
-      <c r="G7" t="inlineStr"/>
-      <c r="H7" t="inlineStr"/>
-      <c r="I7" t="inlineStr"/>
-      <c r="J7" t="inlineStr"/>
-      <c r="K7" t="inlineStr"/>
-      <c r="L7" t="inlineStr"/>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr"/>
-      <c r="B8" t="inlineStr"/>
-      <c r="C8" t="inlineStr"/>
-      <c r="D8" t="inlineStr"/>
-      <c r="E8" t="inlineStr"/>
-      <c r="F8" t="inlineStr"/>
-      <c r="G8" t="inlineStr"/>
-      <c r="H8" t="inlineStr"/>
-      <c r="I8" t="inlineStr"/>
-      <c r="J8" t="inlineStr"/>
-      <c r="K8" t="inlineStr"/>
-      <c r="L8" t="inlineStr"/>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr"/>
-      <c r="B9" t="inlineStr"/>
-      <c r="C9" t="inlineStr"/>
-      <c r="D9" t="inlineStr"/>
-      <c r="E9" t="inlineStr"/>
-      <c r="F9" t="inlineStr"/>
-      <c r="G9" t="inlineStr"/>
-      <c r="H9" t="inlineStr"/>
-      <c r="I9" t="inlineStr"/>
-      <c r="J9" t="inlineStr"/>
-      <c r="K9" t="inlineStr"/>
-      <c r="L9" t="inlineStr"/>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr"/>
-      <c r="B10" t="inlineStr"/>
-      <c r="C10" t="inlineStr"/>
-      <c r="D10" t="inlineStr"/>
-      <c r="E10" t="inlineStr"/>
-      <c r="F10" t="inlineStr"/>
-      <c r="G10" t="inlineStr"/>
-      <c r="H10" t="inlineStr"/>
-      <c r="I10" t="inlineStr"/>
-      <c r="J10" t="inlineStr"/>
-      <c r="K10" t="inlineStr"/>
-      <c r="L10" t="inlineStr"/>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr"/>
-      <c r="B11" t="inlineStr"/>
-      <c r="C11" t="inlineStr"/>
-      <c r="D11" t="inlineStr"/>
-      <c r="E11" t="inlineStr"/>
-      <c r="F11" t="inlineStr"/>
-      <c r="G11" t="inlineStr"/>
-      <c r="H11" t="inlineStr"/>
-      <c r="I11" t="inlineStr"/>
-      <c r="J11" t="inlineStr"/>
-      <c r="K11" t="inlineStr"/>
-      <c r="L11" t="inlineStr"/>
-    </row>
-    <row r="12">
-      <c r="A12" t="inlineStr"/>
-      <c r="B12" t="inlineStr"/>
-      <c r="C12" t="inlineStr"/>
-      <c r="D12" t="inlineStr"/>
-      <c r="E12" t="inlineStr"/>
-      <c r="F12" t="inlineStr"/>
-      <c r="G12" t="inlineStr"/>
-      <c r="H12" t="inlineStr"/>
-      <c r="I12" t="inlineStr"/>
-      <c r="J12" t="inlineStr"/>
-      <c r="K12" t="inlineStr"/>
-      <c r="L12" t="inlineStr"/>
-    </row>
+    <row r="2"/>
+    <row r="3"/>
+    <row r="4"/>
+    <row r="5"/>
+    <row r="6"/>
+    <row r="7"/>
+    <row r="8"/>
+    <row r="9"/>
+    <row r="10"/>
+    <row r="11"/>
+    <row r="12"/>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
@@ -883,39 +575,17 @@
         </is>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" t="inlineStr"/>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr"/>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr"/>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr"/>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr"/>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr"/>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr"/>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr"/>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr"/>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr"/>
-    </row>
-    <row r="12">
-      <c r="A12" t="inlineStr"/>
-    </row>
+    <row r="2"/>
+    <row r="3"/>
+    <row r="4"/>
+    <row r="5"/>
+    <row r="6"/>
+    <row r="7"/>
+    <row r="8"/>
+    <row r="9"/>
+    <row r="10"/>
+    <row r="11"/>
+    <row r="12"/>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>